<commit_message>
ejercicio para excel estadísticas
</commit_message>
<xml_diff>
--- a/AGE(OPE2017)/EJERCICIOS/EXCEL 2010/00 archivos/11 - FUNCIONES DE ESTADÍSTICA/e2010_fun_est_03.xlsx
+++ b/AGE(OPE2017)/EJERCICIOS/EXCEL 2010/00 archivos/11 - FUNCIONES DE ESTADÍSTICA/e2010_fun_est_03.xlsx
@@ -7,10 +7,13 @@
     <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="ESTADÍSITICA RES" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="TOTAL_PRUEBAS">'ESTADÍSITICA RES'!$D$4:$D$28</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -138,23 +141,23 @@
     <t>Aprobado 3º</t>
   </si>
   <si>
-    <t>La nota que aparece con más frecuencia</t>
-  </si>
-  <si>
-    <t>La nota total de los situados en la posición</t>
-  </si>
-  <si>
     <t>Realizar la suma del TOTAL PRUEBAS redondeado a tres decimales</t>
   </si>
   <si>
     <t>Promedio (Total pruebas) de los que están por encima del promedio</t>
+  </si>
+  <si>
+    <t>La posición ocupada a partir de la nota Total Pruebas</t>
+  </si>
+  <si>
+    <t>La nota que aparece con más frecuencia en cada prueba</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +169,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -184,7 +195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -207,18 +218,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Cálculo" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Salida" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -520,7 +549,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -568,10 +597,7 @@
       <c r="C4">
         <v>43.94</v>
       </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D28" si="0">ROUND(B4+C4,3)</f>
-        <v>87.53</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="G4">
         <v>2</v>
       </c>
@@ -589,10 +615,7 @@
       <c r="C5">
         <v>37.020000000000003</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>81.319999999999993</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="J5" t="s">
         <v>32</v>
       </c>
@@ -608,10 +631,7 @@
       <c r="C6">
         <v>42.37</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>80.31</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="J6" t="s">
         <v>33</v>
       </c>
@@ -627,10 +647,7 @@
       <c r="C7">
         <v>44.45</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>79.44</v>
-      </c>
+      <c r="D7" s="2"/>
       <c r="J7" t="s">
         <v>34</v>
       </c>
@@ -646,10 +663,7 @@
       <c r="C8">
         <v>41.41</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>78.14</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="G8">
         <v>3</v>
       </c>
@@ -667,10 +681,7 @@
       <c r="C9">
         <v>35.700000000000003</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>78.11</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="J9" t="s">
         <v>32</v>
       </c>
@@ -686,10 +697,7 @@
       <c r="C10">
         <v>38.21</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>77.31</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="J10" t="s">
         <v>33</v>
       </c>
@@ -705,10 +713,7 @@
       <c r="C11">
         <v>36.299999999999997</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>76.52</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="J11" t="s">
         <v>34</v>
       </c>
@@ -724,10 +729,7 @@
       <c r="C12">
         <v>34.770000000000003</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>76.489999999999995</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="G12">
         <v>4</v>
       </c>
@@ -745,10 +747,7 @@
       <c r="C13">
         <v>36.71</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>75.89</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="J13" t="s">
         <v>38</v>
       </c>
@@ -764,10 +763,7 @@
       <c r="C14">
         <v>38.51</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>75.67</v>
-      </c>
+      <c r="D14" s="2"/>
       <c r="J14" t="s">
         <v>37</v>
       </c>
@@ -783,10 +779,7 @@
       <c r="C15">
         <v>39.75</v>
       </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>75.31</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="J15" t="s">
         <v>39</v>
       </c>
@@ -802,15 +795,12 @@
       <c r="C16">
         <v>32.28</v>
       </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>74.39</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="G16">
         <v>5</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -823,10 +813,7 @@
       <c r="C17">
         <v>41.24</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>74.28</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="J17">
         <v>75.89</v>
       </c>
@@ -842,10 +829,7 @@
       <c r="C18">
         <v>36.229999999999997</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>73.89</v>
-      </c>
+      <c r="D18" s="2"/>
       <c r="J18">
         <v>73.89</v>
       </c>
@@ -861,10 +845,7 @@
       <c r="C19">
         <v>34.04</v>
       </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>73.61</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="J19">
         <v>70.650000000000006</v>
       </c>
@@ -880,15 +861,12 @@
       <c r="C20">
         <v>35.950000000000003</v>
       </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>73.58</v>
-      </c>
+      <c r="D20" s="2"/>
       <c r="G20">
         <v>6</v>
       </c>
       <c r="H20" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -901,10 +879,7 @@
       <c r="C21">
         <v>34.479999999999997</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>73.08</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="J21" t="s">
         <v>32</v>
       </c>
@@ -920,10 +895,7 @@
       <c r="C22">
         <v>36.380000000000003</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>71.900000000000006</v>
-      </c>
+      <c r="D22" s="2"/>
       <c r="J22" t="s">
         <v>33</v>
       </c>
@@ -939,10 +911,7 @@
       <c r="C23">
         <v>28.13</v>
       </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>71.77</v>
-      </c>
+      <c r="D23" s="2"/>
       <c r="J23" t="s">
         <v>34</v>
       </c>
@@ -958,15 +927,12 @@
       <c r="C24">
         <v>31.12</v>
       </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>71.42</v>
-      </c>
+      <c r="D24" s="2"/>
       <c r="G24">
         <v>7</v>
       </c>
       <c r="H24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -979,10 +945,7 @@
       <c r="C25">
         <v>32.32</v>
       </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>71.23</v>
-      </c>
+      <c r="D25" s="2"/>
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -995,10 +958,7 @@
       <c r="C26">
         <v>35.5</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>71.05</v>
-      </c>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1010,10 +970,7 @@
       <c r="C27">
         <v>30.71</v>
       </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>70.900000000000006</v>
-      </c>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1025,10 +982,7 @@
       <c r="C28">
         <v>31.1</v>
       </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
-        <v>70.650000000000006</v>
-      </c>
+      <c r="D28" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A4:D28">

</xml_diff>